<commit_message>
Atualização das leituras e apresentações de artigos científicos
</commit_message>
<xml_diff>
--- a/Bibliografia/Listagem 1.xlsx
+++ b/Bibliografia/Listagem 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/27a8628a50772066/R/ICSAP/Bbliografia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/27a8628a50772066/R/ICSAP/Bibliografia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="892" documentId="8_{A970F4A6-B25B-4E0A-B438-2B0FA64B278E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F8BEF0A9-BD71-4049-B0E1-048AD1418D15}"/>
+  <xr:revisionPtr revIDLastSave="895" documentId="8_{A970F4A6-B25B-4E0A-B438-2B0FA64B278E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C2F79E2C-F8C8-48AF-9022-8C859DBA7627}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{92966055-116D-42DB-900B-B75A724BA527}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3420" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3421" uniqueCount="337">
   <si>
     <t>Palavra-chave</t>
   </si>
@@ -1100,6 +1100,12 @@
   </si>
   <si>
     <t>1) Estudo descritivo ecológico</t>
+  </si>
+  <si>
+    <t>1) Médias móveis trienais
+2) Regressão de Poisson
+3) testada a sobredispersão dos dados (comando poisgof)
+4) Regressão binomial negativa</t>
   </si>
 </sst>
 </file>
@@ -1599,7 +1605,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2194,7 +2200,7 @@
       </c>
       <c r="K17" s="15"/>
     </row>
-    <row r="18" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="72" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>7</v>
       </c>
@@ -2219,7 +2225,9 @@
       <c r="H18" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I18" s="16"/>
+      <c r="I18" s="16" t="s">
+        <v>336</v>
+      </c>
       <c r="J18" s="18" t="s">
         <v>48</v>
       </c>

</xml_diff>